<commit_message>
import excel to update kanban
</commit_message>
<xml_diff>
--- a/pms-server/uploadfiles/template/kanban.xlsx
+++ b/pms-server/uploadfiles/template/kanban.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqi/projects/work/pms/pms-server/uploadfiles/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nr</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Remark</t>
   </si>
   <si>
-    <t>Wire Nr</t>
-  </si>
-  <si>
     <t>Product Nr</t>
   </si>
   <si>
@@ -68,17 +65,33 @@
     <t>Process List</t>
   </si>
   <si>
-    <t>Operate</t>
+    <t>Operator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,13 +114,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,12 +462,10 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>